<commit_message>
Finalmente?? Acho que não
</commit_message>
<xml_diff>
--- a/UC_CBD_GRUPO1/UC_CBD_GRUPO1_FASE_2/plano_de_tarefas.xlsx
+++ b/UC_CBD_GRUPO1/UC_CBD_GRUPO1_FASE_2/plano_de_tarefas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aletorres\Desktop\Complementos Base De Dados\ProjetoComplementos\UC_CBD_GRUPO1\bd projeto\UC_CBD_GRUPO1_FASE2_Funcional\UC_CBD_GRUPO1_FASE2_Funcional_Gaybriel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aletorres\Desktop\Complementos Base De Dados\ProjetoComplementos\UC_CBD_GRUPO1\UC_CBD_GRUPO1_FASE_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD35431-D34B-453C-BB60-C8788EB3708A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A30ADF-60DA-40D2-8646-401DC57E5965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -117,10 +117,6 @@
     <t>Tarefa_9</t>
   </si>
   <si>
-    <t>Definição de potenciais índices e utilização de “
-hints ” para melhorar a performance do</t>
-  </si>
-  <si>
     <t>Tarefa_10</t>
   </si>
   <si>
@@ -159,9 +155,6 @@
   </si>
   <si>
     <t>Tarefa_19</t>
-  </si>
-  <si>
-    <t>implementar uma tabela que permita validar os códigos postaois</t>
   </si>
   <si>
     <t>Modelo de entidade e relacionamento</t>
@@ -205,6 +198,13 @@
   </si>
   <si>
     <t>não</t>
+  </si>
+  <si>
+    <t>Definição de potenciais índices e utilização de “
+hints ” para melhorar a performance da base de dados</t>
+  </si>
+  <si>
+    <t>implementar uma tabela que permita validar o código postal, o concelho e o distrito</t>
   </si>
 </sst>
 </file>
@@ -614,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,7 +643,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -717,7 +717,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E6" s="5">
         <v>2</v>
@@ -731,7 +731,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>8</v>
@@ -745,10 +745,10 @@
         <v>18</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>8</v>
@@ -765,10 +765,10 @@
         <v>20</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E9" s="5">
         <v>3</v>
@@ -782,7 +782,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>8</v>
@@ -796,13 +796,13 @@
         <v>23</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E11" s="5">
         <v>3</v>
@@ -810,16 +810,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>26</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E12" s="5">
         <v>3</v>
@@ -827,16 +827,16 @@
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="C13" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E13" s="5">
         <v>3</v>
@@ -844,16 +844,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>30</v>
-      </c>
       <c r="C14" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E14" s="5">
         <v>3</v>
@@ -861,13 +861,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>8</v>
@@ -878,16 +878,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E16" s="5">
         <v>3</v>
@@ -895,13 +895,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>8</v>
@@ -912,13 +912,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>8</v>
@@ -929,13 +929,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>8</v>
@@ -946,13 +946,13 @@
     </row>
     <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>8</v>
@@ -963,13 +963,13 @@
     </row>
     <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>8</v>

</xml_diff>